<commit_message>
Added data and downloader
</commit_message>
<xml_diff>
--- a/DATA/ChIP_Source_Data_Manifest.xlsx
+++ b/DATA/ChIP_Source_Data_Manifest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/work/ELT-2-ChIP-revision/DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04BED76B-5F8E-4747-BD9C-B18A9C26D0E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0984DB07-CDA9-484A-8582-B7D176AFFB59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1460" windowWidth="31020" windowHeight="16540" xr2:uid="{24B02A36-9EE1-A74E-A7BD-5584D5091E13}"/>
+    <workbookView xWindow="0" yWindow="1460" windowWidth="28800" windowHeight="16540" xr2:uid="{24B02A36-9EE1-A74E-A7BD-5584D5091E13}"/>
   </bookViews>
   <sheets>
     <sheet name="modENCODE data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="96">
   <si>
     <t>https://www.encodeproject.org/files/ENCFF326DPS/@@download/ENCFF326DPS.bigWig?proxy=true</t>
   </si>
@@ -112,9 +112,6 @@
     <t>https://www.encodeproject.org/files/ENCFF578BBV/@@download/ENCFF578BBV.bigBed?proxy=true</t>
   </si>
   <si>
-    <t>DVE-1</t>
-  </si>
-  <si>
     <t>https://www.encodeproject.org/files/ENCFF254ODT/@@download/ENCFF254ODT.bigWig?proxy=true</t>
   </si>
   <si>
@@ -196,9 +193,6 @@
     <t>https://epic.gs.washington.edu/expts/20090415_egl-27b_1_L1.html#tree</t>
   </si>
   <si>
-    <t>Egl-27</t>
-  </si>
-  <si>
     <t>Combined Subtracted dve-1 late embryonic</t>
   </si>
   <si>
@@ -217,9 +211,6 @@
     <t>NHR2_ME_rep1_subtracted.bw</t>
   </si>
   <si>
-    <t>NHR-2</t>
-  </si>
-  <si>
     <t>Mixed-stage Embryo</t>
   </si>
   <si>
@@ -250,9 +241,6 @@
     <t>https://www.encodeproject.org/files/ENCFF512UKH/@@download/ENCFF512UKH.bigBed?proxy=true</t>
   </si>
   <si>
-    <t>PHA-4</t>
-  </si>
-  <si>
     <t>https://www.encodeproject.org/files/ENCFF398QZX/@@download/ENCFF398QZX.bigWig?proxy=true</t>
   </si>
   <si>
@@ -286,9 +274,6 @@
     <t>https://www.encodeproject.org/files/ENCFF939LKU/@@download/ENCFF939LKU.bigBed?proxy=true</t>
   </si>
   <si>
-    <t>SMA-9</t>
-  </si>
-  <si>
     <t>L2 only</t>
   </si>
   <si>
@@ -320,6 +305,24 @@
   </si>
   <si>
     <t>TDP-1</t>
+  </si>
+  <si>
+    <t>#ELT-2</t>
+  </si>
+  <si>
+    <t>#DVE-1</t>
+  </si>
+  <si>
+    <t>#PHA-4</t>
+  </si>
+  <si>
+    <t>#SMA-9</t>
+  </si>
+  <si>
+    <t>#Egl-27</t>
+  </si>
+  <si>
+    <t>#NHR-2</t>
   </si>
 </sst>
 </file>
@@ -729,7 +732,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -764,12 +767,12 @@
         <v>17</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>90</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>13</v>
@@ -784,7 +787,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>0</v>
@@ -807,7 +810,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>2</v>
@@ -815,7 +818,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>90</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
@@ -830,7 +833,7 @@
         <v>4</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>5</v>
@@ -853,7 +856,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>7</v>
@@ -861,7 +864,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>90</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>13</v>
@@ -876,7 +879,7 @@
         <v>23</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>24</v>
@@ -884,12 +887,12 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>13</v>
@@ -901,21 +904,21 @@
         <v>19</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>13</v>
@@ -927,18 +930,18 @@
         <v>19</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>13</v>
@@ -950,18 +953,18 @@
         <v>19</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="G10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>13</v>
@@ -973,18 +976,18 @@
         <v>20</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="G11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>13</v>
@@ -996,18 +999,18 @@
         <v>19</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>13</v>
@@ -1019,18 +1022,18 @@
         <v>19</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>13</v>
@@ -1042,18 +1045,18 @@
         <v>19</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>13</v>
@@ -1068,10 +1071,10 @@
         <v>6</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1083,34 +1086,34 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>14</v>
@@ -1119,21 +1122,21 @@
         <v>19</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>15</v>
@@ -1142,21 +1145,21 @@
         <v>19</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F21" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>16</v>
@@ -1165,21 +1168,21 @@
         <v>19</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>20</v>
@@ -1188,10 +1191,10 @@
         <v>6</v>
       </c>
       <c r="F23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1215,76 +1218,76 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>